<commit_message>
ajustes do acento, e exception
</commit_message>
<xml_diff>
--- a/lost-and-found/parser-quiz/input.xlsx
+++ b/lost-and-found/parser-quiz/input.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="646">
   <si>
     <t>ID Bloco</t>
   </si>
@@ -1110,6 +1110,12 @@
   </si>
   <si>
     <t xml:space="preserve">Tanto na rede privada quanto no SUS, as equipes de saúde são, por lei, obrigadas a denunciar à polícia casos de violência contra a mulher. A depender da condição, uma visita de rotina pode te ajudar a romper o ciclo de violência. </t>
+  </si>
+  <si>
+    <t>R98</t>
+  </si>
+  <si>
+    <t>XXXX</t>
   </si>
   <si>
     <t>ID Resposta</t>
@@ -13182,10 +13188,18 @@
       <c r="Z98" s="6"/>
     </row>
     <row r="99" ht="12.75" customHeight="1">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="6"/>
+      <c r="A99" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>339</v>
+      </c>
       <c r="E99" s="6"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
@@ -38361,19 +38375,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -38402,13 +38416,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E2" s="48" t="s">
         <v>3</v>
@@ -38441,13 +38455,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E3" s="52" t="s">
         <v>3</v>
@@ -38480,13 +38494,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D4" s="56" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E4" s="57" t="s">
         <v>3</v>
@@ -38519,13 +38533,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E5" s="60" t="s">
         <v>5</v>
@@ -38558,13 +38572,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="64" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D6" s="66" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E6" s="64" t="s">
         <v>11</v>
@@ -38597,13 +38611,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="68" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C7" s="69" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E7" s="68" t="s">
         <v>5</v>
@@ -38636,13 +38650,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C8" s="65" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E8" s="64" t="s">
         <v>11</v>
@@ -38675,13 +38689,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="64" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D9" s="66" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E9" s="64" t="s">
         <v>11</v>
@@ -38714,19 +38728,19 @@
         <v>5</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C10" s="69" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D10" s="70" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E10" s="68" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="71" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="G10" s="70"/>
       <c r="H10" s="70"/>
@@ -38755,13 +38769,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="68" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C11" s="69" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E11" s="68" t="s">
         <v>5</v>
@@ -38794,13 +38808,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="68" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C12" s="69" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D12" s="70" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E12" s="68" t="s">
         <v>5</v>
@@ -38833,13 +38847,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C13" s="69" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D13" s="70" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="E13" s="68" t="s">
         <v>5</v>
@@ -38875,10 +38889,10 @@
         <v>168</v>
       </c>
       <c r="C14" s="69" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D14" s="70" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="E14" s="68" t="s">
         <v>5</v>
@@ -38914,10 +38928,10 @@
         <v>177</v>
       </c>
       <c r="C15" s="69" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D15" s="70" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E15" s="68" t="s">
         <v>5</v>
@@ -38953,10 +38967,10 @@
         <v>177</v>
       </c>
       <c r="C16" s="69" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D16" s="70" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="E16" s="68" t="s">
         <v>5</v>
@@ -38992,10 +39006,10 @@
         <v>177</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D17" s="72" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E17" s="68" t="s">
         <v>5</v>
@@ -39028,13 +39042,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C18" s="69" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D18" s="73" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E18" s="68" t="s">
         <v>5</v>
@@ -39067,13 +39081,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C19" s="69" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D19" s="70" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E19" s="68" t="s">
         <v>5</v>
@@ -39109,10 +39123,10 @@
         <v>185</v>
       </c>
       <c r="C20" s="69" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D20" s="70" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E20" s="68" t="s">
         <v>5</v>
@@ -39145,13 +39159,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C21" s="69" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D21" s="70" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E21" s="68" t="s">
         <v>5</v>
@@ -39187,10 +39201,10 @@
         <v>185</v>
       </c>
       <c r="C22" s="69" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D22" s="70" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E22" s="68" t="s">
         <v>5</v>
@@ -39226,10 +39240,10 @@
         <v>186</v>
       </c>
       <c r="C23" s="69" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D23" s="70" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E23" s="68" t="s">
         <v>5</v>
@@ -39262,13 +39276,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="68" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C24" s="69" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D24" s="70" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E24" s="68" t="s">
         <v>5</v>
@@ -39301,13 +39315,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="68" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C25" s="69" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D25" s="74" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E25" s="68" t="s">
         <v>5</v>
@@ -39340,13 +39354,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="68" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C26" s="69" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D26" s="70" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="E26" s="68" t="s">
         <v>5</v>
@@ -39379,13 +39393,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="76" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C27" s="77" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D27" s="78" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="E27" s="68" t="s">
         <v>5</v>
@@ -39421,10 +39435,10 @@
         <v>187</v>
       </c>
       <c r="C28" s="81" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D28" s="82" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="E28" s="80" t="s">
         <v>13</v>
@@ -39460,10 +39474,10 @@
         <v>187</v>
       </c>
       <c r="C29" s="85" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D29" s="86" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="E29" s="84" t="s">
         <v>13</v>
@@ -39496,13 +39510,13 @@
         <v>13</v>
       </c>
       <c r="B30" s="84" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C30" s="85" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D30" s="86" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E30" s="84" t="s">
         <v>13</v>
@@ -39535,13 +39549,13 @@
         <v>13</v>
       </c>
       <c r="B31" s="84" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C31" s="85" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D31" s="86" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="E31" s="84" t="s">
         <v>13</v>
@@ -39577,10 +39591,10 @@
         <v>189</v>
       </c>
       <c r="C32" s="85" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D32" s="86" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="E32" s="84" t="s">
         <v>13</v>
@@ -39616,10 +39630,10 @@
         <v>189</v>
       </c>
       <c r="C33" s="85" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D33" s="86" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="E33" s="84" t="s">
         <v>13</v>
@@ -39655,10 +39669,10 @@
         <v>189</v>
       </c>
       <c r="C34" s="85" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D34" s="86" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="E34" s="84" t="s">
         <v>13</v>
@@ -39694,10 +39708,10 @@
         <v>189</v>
       </c>
       <c r="C35" s="85" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D35" s="86" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="E35" s="84" t="s">
         <v>13</v>
@@ -39733,10 +39747,10 @@
         <v>189</v>
       </c>
       <c r="C36" s="85" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="D36" s="87" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="E36" s="84" t="s">
         <v>13</v>
@@ -39772,10 +39786,10 @@
         <v>189</v>
       </c>
       <c r="C37" s="85" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D37" s="86" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E37" s="84" t="s">
         <v>13</v>
@@ -39811,10 +39825,10 @@
         <v>191</v>
       </c>
       <c r="C38" s="85" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D38" s="86" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="E38" s="84" t="s">
         <v>13</v>
@@ -39850,10 +39864,10 @@
         <v>191</v>
       </c>
       <c r="C39" s="85" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D39" s="86" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E39" s="84" t="s">
         <v>13</v>
@@ -39889,10 +39903,10 @@
         <v>191</v>
       </c>
       <c r="C40" s="85" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D40" s="86" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="E40" s="84" t="s">
         <v>13</v>
@@ -39928,10 +39942,10 @@
         <v>191</v>
       </c>
       <c r="C41" s="85" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D41" s="86" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="E41" s="84" t="s">
         <v>13</v>
@@ -39967,10 +39981,10 @@
         <v>193</v>
       </c>
       <c r="C42" s="85" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D42" s="86" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E42" s="84" t="s">
         <v>13</v>
@@ -40006,10 +40020,10 @@
         <v>193</v>
       </c>
       <c r="C43" s="85" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D43" s="86" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="E43" s="84" t="s">
         <v>13</v>
@@ -40045,10 +40059,10 @@
         <v>193</v>
       </c>
       <c r="C44" s="85" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D44" s="86" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="E44" s="84" t="s">
         <v>13</v>
@@ -40084,10 +40098,10 @@
         <v>195</v>
       </c>
       <c r="C45" s="85" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D45" s="86" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="E45" s="84" t="s">
         <v>13</v>
@@ -40123,10 +40137,10 @@
         <v>195</v>
       </c>
       <c r="C46" s="85" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D46" s="86" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="E46" s="84" t="s">
         <v>13</v>
@@ -40162,10 +40176,10 @@
         <v>195</v>
       </c>
       <c r="C47" s="85" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D47" s="86" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="E47" s="84" t="s">
         <v>13</v>
@@ -40201,10 +40215,10 @@
         <v>199</v>
       </c>
       <c r="C48" s="90" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D48" s="91" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="E48" s="89" t="s">
         <v>13</v>
@@ -40240,10 +40254,10 @@
         <v>203</v>
       </c>
       <c r="C49" s="93" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="E49" s="92" t="s">
         <v>7</v>
@@ -40279,10 +40293,10 @@
         <v>203</v>
       </c>
       <c r="C50" s="93" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="E50" s="92" t="s">
         <v>7</v>
@@ -40318,10 +40332,10 @@
         <v>203</v>
       </c>
       <c r="C51" s="92" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="E51" s="92" t="s">
         <v>7</v>
@@ -40357,10 +40371,10 @@
         <v>203</v>
       </c>
       <c r="C52" s="92" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E52" s="92" t="s">
         <v>7</v>
@@ -40393,13 +40407,13 @@
         <v>7</v>
       </c>
       <c r="B53" s="92" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C53" s="92" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E53" s="92" t="s">
         <v>7</v>
@@ -40435,10 +40449,10 @@
         <v>209</v>
       </c>
       <c r="C54" s="92" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E54" s="92" t="s">
         <v>7</v>
@@ -40471,13 +40485,13 @@
         <v>7</v>
       </c>
       <c r="B55" s="92" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C55" s="92" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E55" s="92" t="s">
         <v>7</v>
@@ -40513,10 +40527,10 @@
         <v>209</v>
       </c>
       <c r="C56" s="92" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E56" s="92" t="s">
         <v>7</v>
@@ -40549,13 +40563,13 @@
         <v>7</v>
       </c>
       <c r="B57" s="94" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C57" s="94" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D57" s="95" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="E57" s="94" t="s">
         <v>11</v>
@@ -40588,13 +40602,13 @@
         <v>7</v>
       </c>
       <c r="B58" s="94" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C58" s="94" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D58" s="95" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E58" s="94" t="s">
         <v>11</v>
@@ -40627,13 +40641,13 @@
         <v>7</v>
       </c>
       <c r="B59" s="94" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C59" s="94" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D59" s="95" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E59" s="94" t="s">
         <v>11</v>
@@ -40669,10 +40683,10 @@
         <v>209</v>
       </c>
       <c r="C60" s="92" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E60" s="92" t="s">
         <v>7</v>
@@ -40705,13 +40719,13 @@
         <v>7</v>
       </c>
       <c r="B61" s="92" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C61" s="92" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E61" s="92" t="s">
         <v>7</v>
@@ -40744,13 +40758,13 @@
         <v>7</v>
       </c>
       <c r="B62" s="96" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C62" s="96" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D62" s="97" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E62" s="96" t="s">
         <v>7</v>
@@ -40783,13 +40797,13 @@
         <v>7</v>
       </c>
       <c r="B63" s="92" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C63" s="92" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D63" s="98" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E63" s="92" t="s">
         <v>7</v>
@@ -40825,10 +40839,10 @@
         <v>221</v>
       </c>
       <c r="C64" s="92" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E64" s="92" t="s">
         <v>7</v>
@@ -40864,10 +40878,10 @@
         <v>221</v>
       </c>
       <c r="C65" s="92" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="E65" s="92" t="s">
         <v>7</v>
@@ -40903,10 +40917,10 @@
         <v>221</v>
       </c>
       <c r="C66" s="92" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="E66" s="92" t="s">
         <v>7</v>
@@ -40942,10 +40956,10 @@
         <v>225</v>
       </c>
       <c r="C67" s="92" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D67" s="98" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="E67" s="92" t="s">
         <v>7</v>
@@ -40981,10 +40995,10 @@
         <v>225</v>
       </c>
       <c r="C68" s="99" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E68" s="92" t="s">
         <v>7</v>
@@ -41020,10 +41034,10 @@
         <v>225</v>
       </c>
       <c r="C69" s="92" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="E69" s="92" t="s">
         <v>7</v>
@@ -41059,10 +41073,10 @@
         <v>225</v>
       </c>
       <c r="C70" s="99" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="E70" s="92" t="s">
         <v>7</v>
@@ -41095,13 +41109,13 @@
         <v>7</v>
       </c>
       <c r="B71" s="92" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C71" s="99" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="E71" s="92" t="s">
         <v>7</v>
@@ -41134,13 +41148,13 @@
         <v>7</v>
       </c>
       <c r="B72" s="92" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C72" s="99" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E72" s="92" t="s">
         <v>7</v>
@@ -41173,13 +41187,13 @@
         <v>7</v>
       </c>
       <c r="B73" s="92" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C73" s="99" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="E73" s="92" t="s">
         <v>7</v>
@@ -41212,13 +41226,13 @@
         <v>7</v>
       </c>
       <c r="B74" s="92" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C74" s="92" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="E74" s="92" t="s">
         <v>7</v>
@@ -41254,10 +41268,10 @@
         <v>241</v>
       </c>
       <c r="C75" s="92" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E75" s="92" t="s">
         <v>7</v>
@@ -41293,10 +41307,10 @@
         <v>241</v>
       </c>
       <c r="C76" s="92" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E76" s="92" t="s">
         <v>7</v>
@@ -41329,13 +41343,13 @@
         <v>7</v>
       </c>
       <c r="B77" s="92" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C77" s="92" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="E77" s="92" t="s">
         <v>7</v>
@@ -41368,13 +41382,13 @@
         <v>7</v>
       </c>
       <c r="B78" s="92" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C78" s="92" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E78" s="92" t="s">
         <v>7</v>
@@ -41407,13 +41421,13 @@
         <v>7</v>
       </c>
       <c r="B79" s="96" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C79" s="96" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="D79" s="97" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E79" s="96" t="s">
         <v>7</v>
@@ -41449,10 +41463,10 @@
         <v>264</v>
       </c>
       <c r="C80" s="100" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D80" s="101" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E80" s="100" t="s">
         <v>9</v>
@@ -41485,13 +41499,13 @@
         <v>9</v>
       </c>
       <c r="B81" s="100" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C81" s="100" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D81" s="101" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="E81" s="100" t="s">
         <v>9</v>
@@ -41524,13 +41538,13 @@
         <v>9</v>
       </c>
       <c r="B82" s="100" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C82" s="100" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D82" s="101" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E82" s="100" t="s">
         <v>9</v>
@@ -41563,13 +41577,13 @@
         <v>9</v>
       </c>
       <c r="B83" s="100" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C83" s="100" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="D83" s="101" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="E83" s="100" t="s">
         <v>9</v>
@@ -41605,10 +41619,10 @@
         <v>264</v>
       </c>
       <c r="C84" s="100" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D84" s="101" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="E84" s="100" t="s">
         <v>9</v>
@@ -41644,10 +41658,10 @@
         <v>264</v>
       </c>
       <c r="C85" s="100" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="D85" s="101" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="E85" s="100" t="s">
         <v>9</v>
@@ -41680,13 +41694,13 @@
         <v>9</v>
       </c>
       <c r="B86" s="100" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C86" s="100" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="D86" s="101" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E86" s="100" t="s">
         <v>9</v>
@@ -41722,10 +41736,10 @@
         <v>264</v>
       </c>
       <c r="C87" s="100" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="D87" s="101" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="E87" s="100" t="s">
         <v>9</v>
@@ -41761,10 +41775,10 @@
         <v>264</v>
       </c>
       <c r="C88" s="100" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D88" s="102" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E88" s="100" t="s">
         <v>9</v>
@@ -41800,10 +41814,10 @@
         <v>266</v>
       </c>
       <c r="C89" s="100" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="D89" s="101" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="E89" s="100" t="s">
         <v>9</v>
@@ -41839,10 +41853,10 @@
         <v>268</v>
       </c>
       <c r="C90" s="100" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="D90" s="101" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="E90" s="100" t="s">
         <v>9</v>
@@ -41878,10 +41892,10 @@
         <v>268</v>
       </c>
       <c r="C91" s="100" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D91" s="101" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E91" s="100" t="s">
         <v>9</v>
@@ -41914,13 +41928,13 @@
         <v>9</v>
       </c>
       <c r="B92" s="103" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C92" s="103" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D92" s="104" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="E92" s="103" t="s">
         <v>9</v>
@@ -41956,10 +41970,10 @@
         <v>276</v>
       </c>
       <c r="C93" s="103" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D93" s="104" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="E93" s="103" t="s">
         <v>9</v>
@@ -41992,13 +42006,13 @@
         <v>9</v>
       </c>
       <c r="B94" s="103" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="C94" s="103" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="D94" s="104" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="E94" s="103" t="s">
         <v>9</v>
@@ -42034,10 +42048,10 @@
         <v>276</v>
       </c>
       <c r="C95" s="103" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D95" s="104" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="E95" s="103" t="s">
         <v>9</v>
@@ -42070,13 +42084,13 @@
         <v>9</v>
       </c>
       <c r="B96" s="103" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C96" s="103" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="D96" s="104" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="E96" s="103" t="s">
         <v>9</v>
@@ -42109,13 +42123,13 @@
         <v>9</v>
       </c>
       <c r="B97" s="103" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C97" s="103" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D97" s="104" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E97" s="103" t="s">
         <v>9</v>
@@ -42151,10 +42165,10 @@
         <v>282</v>
       </c>
       <c r="C98" s="103" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="D98" s="104" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E98" s="103" t="s">
         <v>9</v>
@@ -42190,10 +42204,10 @@
         <v>288</v>
       </c>
       <c r="C99" s="103" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="D99" s="104" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="E99" s="103" t="s">
         <v>9</v>
@@ -42229,10 +42243,10 @@
         <v>290</v>
       </c>
       <c r="C100" s="103" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="D100" s="104" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E100" s="103" t="s">
         <v>9</v>
@@ -42265,13 +42279,13 @@
         <v>9</v>
       </c>
       <c r="B101" s="103" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C101" s="103" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="D101" s="104" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="E101" s="103" t="s">
         <v>9</v>
@@ -42307,10 +42321,10 @@
         <v>290</v>
       </c>
       <c r="C102" s="103" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="D102" s="104" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="E102" s="103" t="s">
         <v>9</v>
@@ -42343,13 +42357,13 @@
         <v>9</v>
       </c>
       <c r="B103" s="105" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C103" s="105" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="D103" s="106" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="E103" s="105" t="s">
         <v>9</v>
@@ -42385,10 +42399,10 @@
         <v>300</v>
       </c>
       <c r="C104" s="64" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D104" s="107" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="E104" s="64" t="s">
         <v>11</v>
@@ -42424,10 +42438,10 @@
         <v>304</v>
       </c>
       <c r="C105" s="64" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="D105" s="107" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="E105" s="64" t="s">
         <v>11</v>
@@ -42463,10 +42477,10 @@
         <v>304</v>
       </c>
       <c r="C106" s="64" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="D106" s="107" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="E106" s="64" t="s">
         <v>11</v>
@@ -42502,10 +42516,10 @@
         <v>304</v>
       </c>
       <c r="C107" s="64" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="D107" s="107" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="E107" s="64" t="s">
         <v>11</v>
@@ -42541,10 +42555,10 @@
         <v>304</v>
       </c>
       <c r="C108" s="64" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="D108" s="107" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="E108" s="64" t="s">
         <v>11</v>
@@ -42580,10 +42594,10 @@
         <v>304</v>
       </c>
       <c r="C109" s="64" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="D109" s="107" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="E109" s="64" t="s">
         <v>11</v>
@@ -42619,10 +42633,10 @@
         <v>304</v>
       </c>
       <c r="C110" s="64" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D110" s="107" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="E110" s="64" t="s">
         <v>11</v>
@@ -42658,10 +42672,10 @@
         <v>304</v>
       </c>
       <c r="C111" s="64" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="D111" s="107" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="E111" s="64" t="s">
         <v>11</v>
@@ -42694,13 +42708,13 @@
         <v>11</v>
       </c>
       <c r="B112" s="64" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C112" s="64" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="D112" s="107" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="E112" s="64" t="s">
         <v>11</v>
@@ -42733,13 +42747,13 @@
         <v>11</v>
       </c>
       <c r="B113" s="64" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C113" s="64" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="D113" s="107" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="E113" s="64" t="s">
         <v>11</v>
@@ -42772,13 +42786,13 @@
         <v>11</v>
       </c>
       <c r="B114" s="64" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C114" s="64" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D114" s="107" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="E114" s="64" t="s">
         <v>11</v>
@@ -42811,13 +42825,13 @@
         <v>11</v>
       </c>
       <c r="B115" s="64" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C115" s="64" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D115" s="107" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="E115" s="64" t="s">
         <v>11</v>
@@ -42850,13 +42864,13 @@
         <v>11</v>
       </c>
       <c r="B116" s="64" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C116" s="64" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="D116" s="107" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="E116" s="64" t="s">
         <v>11</v>
@@ -42889,13 +42903,13 @@
         <v>11</v>
       </c>
       <c r="B117" s="64" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C117" s="64" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D117" s="107" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="E117" s="64" t="s">
         <v>11</v>
@@ -42928,13 +42942,13 @@
         <v>11</v>
       </c>
       <c r="B118" s="64" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C118" s="64" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D118" s="107" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="E118" s="64" t="s">
         <v>11</v>
@@ -42967,13 +42981,13 @@
         <v>11</v>
       </c>
       <c r="B119" s="64" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C119" s="64" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D119" s="107" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="E119" s="64" t="s">
         <v>11</v>
@@ -43006,13 +43020,13 @@
         <v>11</v>
       </c>
       <c r="B120" s="64" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C120" s="64" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D120" s="107" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="E120" s="64" t="s">
         <v>11</v>
@@ -43045,13 +43059,13 @@
         <v>11</v>
       </c>
       <c r="B121" s="64" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C121" s="64" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="D121" s="107" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="E121" s="64" t="s">
         <v>11</v>
@@ -43084,13 +43098,13 @@
         <v>11</v>
       </c>
       <c r="B122" s="64" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C122" s="64" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="D122" s="107" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="E122" s="64" t="s">
         <v>11</v>
@@ -43123,13 +43137,13 @@
         <v>11</v>
       </c>
       <c r="B123" s="64" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C123" s="64" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="D123" s="107" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="E123" s="64" t="s">
         <v>11</v>
@@ -43162,13 +43176,13 @@
         <v>11</v>
       </c>
       <c r="B124" s="64" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C124" s="64" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="D124" s="107" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="E124" s="64" t="s">
         <v>11</v>
@@ -43201,13 +43215,13 @@
         <v>11</v>
       </c>
       <c r="B125" s="64" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C125" s="64" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="D125" s="107" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="E125" s="64" t="s">
         <v>11</v>
@@ -43240,13 +43254,13 @@
         <v>11</v>
       </c>
       <c r="B126" s="64" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="C126" s="64" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="D126" s="107" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="E126" s="64" t="s">
         <v>11</v>
@@ -43282,10 +43296,10 @@
         <v>332</v>
       </c>
       <c r="C127" s="64" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="D127" s="107" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="E127" s="64" t="s">
         <v>11</v>
@@ -43321,10 +43335,10 @@
         <v>332</v>
       </c>
       <c r="C128" s="64" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="D128" s="107" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="E128" s="64" t="s">
         <v>11</v>
@@ -43360,10 +43374,10 @@
         <v>336</v>
       </c>
       <c r="C129" s="64" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="D129" s="107" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="E129" s="64" t="s">
         <v>11</v>
@@ -43399,10 +43413,10 @@
         <v>336</v>
       </c>
       <c r="C130" s="64" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="D130" s="107" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="E130" s="64" t="s">
         <v>11</v>
@@ -43438,10 +43452,10 @@
         <v>336</v>
       </c>
       <c r="C131" s="64" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="D131" s="107" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="E131" s="64" t="s">
         <v>11</v>
@@ -43477,10 +43491,10 @@
         <v>336</v>
       </c>
       <c r="C132" s="64" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D132" s="107" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="E132" s="64" t="s">
         <v>11</v>
@@ -43516,10 +43530,10 @@
         <v>336</v>
       </c>
       <c r="C133" s="64" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="D133" s="107" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="E133" s="64" t="s">
         <v>11</v>
@@ -68487,26 +68501,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update parser.ts para montar o multiplechoice
</commit_message>
<xml_diff>
--- a/lost-and-found/parser-quiz/input.xlsx
+++ b/lost-and-found/parser-quiz/input.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="643">
   <si>
     <t>ID Bloco</t>
   </si>
@@ -102,11 +102,11 @@
     <t>SC</t>
   </si>
   <si>
-    <t>“Passos para fuga”: p0a
+    <t xml:space="preserve">“Passos para fuga”: p0a
 “Crianças, adolescentes e dependentes”, p0b
 “Bens, trabalho e renda”: p0c
 “Segurança pessoal”: p0d
-"Transporte": p0e</t>
+</t>
   </si>
   <si>
     <t>* transporte não pode ser uma das opções de resposta, pq só foi feito o caso especial pro PS, naõ tem o "vai pro transporte só se não foi respondido"</t>
@@ -137,12 +137,6 @@
   </si>
   <si>
     <t>p0d</t>
-  </si>
-  <si>
-    <t>p0e</t>
-  </si>
-  <si>
-    <t>**</t>
   </si>
   <si>
     <t>P1intro</t>
@@ -187,12 +181,12 @@
     <t>Qual deles você quer conhecer?</t>
   </si>
   <si>
+    <t>MC</t>
+  </si>
+  <si>
     <t>“Auxílio-aluguel”: R2, P4
 “Casa abrigo”:  R3, P4
 “Casa de acolhimento”: R4, P4</t>
-  </si>
-  <si>
-    <t>TODO: MC</t>
   </si>
   <si>
     <t>P4</t>
@@ -275,9 +269,6 @@
   </si>
   <si>
     <t>P8ac</t>
-  </si>
-  <si>
-    <t>** vai duplicar aqui se começou pelo transporte **</t>
   </si>
   <si>
     <t>P9intro</t>
@@ -877,7 +868,7 @@
     <t>R57</t>
   </si>
   <si>
-    <t>É dever de todos, especialmente das pessoas mais próximas, denunciar o caso à polícia, ao Ministério Público,  à Justiça ou outro órgão de proteção. Lembre-se que a denúncia pode ser feita de forma anônima.</t>
+    <t>É dever de todos, especialmente das pessoas mais próximas, denunciar o caso à polícia, ao Ministério Público, à Justiça ou outro órgão de proteção. Lembre-se que a denúncia pode ser feita de forma anônima.</t>
   </si>
   <si>
     <t>R58</t>
@@ -1115,7 +1106,7 @@
     <t>R98</t>
   </si>
   <si>
-    <t>XXXX</t>
+    <t xml:space="preserve">Estamos finalizando o bloco "Segurança Pessoal". Obrigada por ter respondido até aqui. Você é forte e corajosa!  O PenhaS quer te ajudar a romper com o ciclo de violência. Certifique-se de todos os itens que aparecerão no seu plano. Eles são personalizados a partir de suas respostas, por isso é tão importante que você siga respondendo a todos os blocos. </t>
   </si>
   <si>
     <t>ID Resposta</t>
@@ -3442,26 +3433,14 @@
       <c r="Z7" s="12"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>39</v>
-      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="14">
-        <v>17.0</v>
-      </c>
+      <c r="H8" s="14"/>
       <c r="I8" s="15"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -3486,13 +3465,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="E9" s="5">
         <v>1.0</v>
@@ -3523,16 +3502,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="F10" s="12"/>
       <c r="H10" s="12"/>
@@ -3560,16 +3539,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
@@ -3598,20 +3577,18 @@
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>54</v>
-      </c>
+      <c r="F12" s="14"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -3638,19 +3615,19 @@
         <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="F13" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>58</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -3678,15 +3655,15 @@
         <v>5</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -3714,16 +3691,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -3752,16 +3729,16 @@
         <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -3790,16 +3767,16 @@
         <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -3828,19 +3805,19 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="F18" s="18" t="s">
         <v>71</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>73</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -3868,16 +3845,14 @@
         <v>5</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="F19" s="13" t="s">
-        <v>75</v>
-      </c>
+      <c r="F19" s="13"/>
       <c r="G19" s="12"/>
       <c r="H19" s="14">
         <v>17.0</v>
@@ -3906,13 +3881,13 @@
         <v>13</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E20" s="5">
         <v>1.0</v>
@@ -3944,16 +3919,16 @@
         <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -3982,13 +3957,13 @@
         <v>7</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E22" s="5">
         <v>1.0</v>
@@ -4020,16 +3995,16 @@
         <v>7</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -4058,16 +4033,16 @@
         <v>7</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -4096,16 +4071,16 @@
         <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -4134,19 +4109,19 @@
         <v>7</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>95</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -4174,16 +4149,16 @@
         <v>7</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -4212,16 +4187,16 @@
         <v>7</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -4250,16 +4225,16 @@
         <v>7</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -4288,16 +4263,16 @@
         <v>7</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -4326,16 +4301,16 @@
         <v>7</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -4364,13 +4339,13 @@
         <v>9</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E32" s="5">
         <v>1.0</v>
@@ -4402,16 +4377,16 @@
         <v>9</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
@@ -4440,16 +4415,16 @@
         <v>9</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
@@ -4478,13 +4453,13 @@
         <v>11</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E35" s="5">
         <v>1.0</v>
@@ -4516,16 +4491,16 @@
         <v>11</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -4554,16 +4529,16 @@
         <v>11</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -4592,16 +4567,16 @@
         <v>11</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -4630,16 +4605,16 @@
         <v>11</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -4668,16 +4643,16 @@
         <v>11</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -4706,16 +4681,16 @@
         <v>11</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -4744,16 +4719,16 @@
         <v>11</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -4810,10 +4785,10 @@
         <v>15</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>15</v>
@@ -9665,16 +9640,16 @@
   <sheetData>
     <row r="1" ht="42.0" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -9704,13 +9679,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -9740,13 +9715,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
@@ -9776,13 +9751,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -9812,13 +9787,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -9848,13 +9823,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -9884,13 +9859,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -9920,13 +9895,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -9956,13 +9931,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -9992,13 +9967,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -10028,13 +10003,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -10064,13 +10039,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -10100,13 +10075,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -10136,13 +10111,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="D14" s="22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -10172,13 +10147,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -10208,13 +10183,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -10244,13 +10219,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -10280,13 +10255,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -10316,13 +10291,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -10352,10 +10327,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="12"/>
@@ -10386,10 +10361,10 @@
         <v>5</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="12"/>
@@ -10420,13 +10395,13 @@
         <v>13</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -10456,13 +10431,13 @@
         <v>13</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -10492,13 +10467,13 @@
         <v>13</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -10528,13 +10503,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -10564,13 +10539,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -10600,13 +10575,13 @@
         <v>13</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -10636,13 +10611,13 @@
         <v>13</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -10672,13 +10647,13 @@
         <v>13</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -10708,13 +10683,13 @@
         <v>7</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -10744,13 +10719,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -10780,13 +10755,13 @@
         <v>7</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
@@ -10816,13 +10791,13 @@
         <v>7</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -10852,13 +10827,13 @@
         <v>7</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -10888,13 +10863,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -10924,13 +10899,13 @@
         <v>7</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -10960,13 +10935,13 @@
         <v>7</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -10996,13 +10971,13 @@
         <v>7</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
@@ -11032,13 +11007,13 @@
         <v>7</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -11068,13 +11043,13 @@
         <v>7</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D40" s="34" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -11104,13 +11079,13 @@
         <v>7</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -11140,13 +11115,13 @@
         <v>7</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D42" s="34" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -11176,13 +11151,13 @@
         <v>7</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
@@ -11212,13 +11187,13 @@
         <v>7</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D44" s="34" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -11248,13 +11223,13 @@
         <v>7</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -11284,13 +11259,13 @@
         <v>7</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D46" s="34" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -11320,13 +11295,13 @@
         <v>7</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -11356,13 +11331,13 @@
         <v>7</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -11392,13 +11367,13 @@
         <v>7</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D49" s="34" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
@@ -11428,13 +11403,13 @@
         <v>7</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -11464,13 +11439,13 @@
         <v>7</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -11500,13 +11475,13 @@
         <v>7</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
@@ -11536,13 +11511,13 @@
         <v>7</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -11572,13 +11547,13 @@
         <v>7</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -11608,13 +11583,13 @@
         <v>7</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -11644,13 +11619,13 @@
         <v>7</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -11680,13 +11655,13 @@
         <v>7</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D57" s="34" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
@@ -11716,13 +11691,13 @@
         <v>7</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -11752,13 +11727,13 @@
         <v>7</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D59" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -11788,13 +11763,13 @@
         <v>7</v>
       </c>
       <c r="B60" s="38" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C60" s="38" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D60" s="39" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
@@ -11824,13 +11799,13 @@
         <v>9</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -11860,13 +11835,13 @@
         <v>9</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
@@ -11896,13 +11871,13 @@
         <v>9</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -11932,13 +11907,13 @@
         <v>9</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -11968,13 +11943,13 @@
         <v>9</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
@@ -12004,13 +11979,13 @@
         <v>9</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -12040,13 +12015,13 @@
         <v>9</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D67" s="41" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
@@ -12076,13 +12051,13 @@
         <v>9</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D68" s="41" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
@@ -12112,13 +12087,13 @@
         <v>9</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D69" s="41" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -12148,13 +12123,13 @@
         <v>9</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D70" s="41" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -12184,13 +12159,13 @@
         <v>9</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D71" s="41" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
@@ -12220,13 +12195,13 @@
         <v>9</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -12256,13 +12231,13 @@
         <v>9</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
@@ -12292,13 +12267,13 @@
         <v>9</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
@@ -12328,13 +12303,13 @@
         <v>9</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D75" s="40" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -12364,13 +12339,13 @@
         <v>9</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
@@ -12400,13 +12375,13 @@
         <v>9</v>
       </c>
       <c r="B77" s="38" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C77" s="38" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D77" s="42" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
@@ -12436,13 +12411,13 @@
         <v>11</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -12472,13 +12447,13 @@
         <v>11</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E79" s="6"/>
       <c r="F79" s="6"/>
@@ -12508,13 +12483,13 @@
         <v>11</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -12544,13 +12519,13 @@
         <v>11</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
@@ -12580,13 +12555,13 @@
         <v>11</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
@@ -12616,13 +12591,13 @@
         <v>11</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
@@ -12652,13 +12627,13 @@
         <v>11</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E84" s="6"/>
       <c r="F84" s="6"/>
@@ -12688,13 +12663,13 @@
         <v>11</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E85" s="6"/>
       <c r="F85" s="6"/>
@@ -12724,13 +12699,13 @@
         <v>11</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E86" s="6"/>
       <c r="F86" s="6"/>
@@ -12760,13 +12735,13 @@
         <v>11</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E87" s="6"/>
       <c r="F87" s="6"/>
@@ -12796,13 +12771,13 @@
         <v>11</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E88" s="6"/>
       <c r="F88" s="6"/>
@@ -12832,13 +12807,13 @@
         <v>11</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E89" s="6"/>
       <c r="F89" s="6"/>
@@ -12868,13 +12843,13 @@
         <v>11</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E90" s="6"/>
       <c r="F90" s="6"/>
@@ -12904,13 +12879,13 @@
         <v>11</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E91" s="6"/>
       <c r="F91" s="6"/>
@@ -12940,13 +12915,13 @@
         <v>11</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E92" s="6"/>
       <c r="F92" s="6"/>
@@ -12976,13 +12951,13 @@
         <v>11</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E93" s="6"/>
       <c r="F93" s="6"/>
@@ -13012,13 +12987,13 @@
         <v>11</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E94" s="6"/>
       <c r="F94" s="6"/>
@@ -13048,13 +13023,13 @@
         <v>11</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E95" s="6"/>
       <c r="F95" s="6"/>
@@ -13084,13 +13059,13 @@
         <v>11</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E96" s="6"/>
       <c r="F96" s="6"/>
@@ -13120,13 +13095,13 @@
         <v>11</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E97" s="6"/>
       <c r="F97" s="6"/>
@@ -13156,13 +13131,13 @@
         <v>11</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E98" s="6"/>
       <c r="F98" s="6"/>
@@ -13192,13 +13167,13 @@
         <v>11</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E99" s="6"/>
       <c r="F99" s="6"/>
@@ -38375,19 +38350,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E1" s="43" t="s">
         <v>340</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>343</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>344</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -38416,13 +38391,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E2" s="48" t="s">
         <v>3</v>
@@ -38455,13 +38430,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="50" t="s">
+        <v>342</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>345</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>348</v>
-      </c>
       <c r="D3" s="51" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E3" s="52" t="s">
         <v>3</v>
@@ -38494,13 +38469,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D4" s="56" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E4" s="57" t="s">
         <v>3</v>
@@ -38533,13 +38508,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E5" s="60" t="s">
         <v>5</v>
@@ -38572,13 +38547,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="64" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D6" s="66" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E6" s="64" t="s">
         <v>11</v>
@@ -38611,13 +38586,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="68" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C7" s="69" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E7" s="68" t="s">
         <v>5</v>
@@ -38650,13 +38625,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C8" s="65" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E8" s="64" t="s">
         <v>11</v>
@@ -38689,13 +38664,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="64" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D9" s="66" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="E9" s="64" t="s">
         <v>11</v>
@@ -38728,19 +38703,19 @@
         <v>5</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C10" s="69" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D10" s="70" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E10" s="68" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="71" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G10" s="70"/>
       <c r="H10" s="70"/>
@@ -38769,13 +38744,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="68" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C11" s="69" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E11" s="68" t="s">
         <v>5</v>
@@ -38808,13 +38783,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="68" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C12" s="69" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D12" s="70" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E12" s="68" t="s">
         <v>5</v>
@@ -38847,13 +38822,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C13" s="69" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D13" s="70" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E13" s="68" t="s">
         <v>5</v>
@@ -38886,13 +38861,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C14" s="69" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D14" s="70" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E14" s="68" t="s">
         <v>5</v>
@@ -38925,13 +38900,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C15" s="69" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D15" s="70" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E15" s="68" t="s">
         <v>5</v>
@@ -38964,13 +38939,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="69" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C16" s="69" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D16" s="70" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E16" s="68" t="s">
         <v>5</v>
@@ -39003,13 +38978,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="69" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D17" s="72" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E17" s="68" t="s">
         <v>5</v>
@@ -39042,13 +39017,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C18" s="69" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D18" s="73" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E18" s="68" t="s">
         <v>5</v>
@@ -39081,13 +39056,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C19" s="69" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D19" s="70" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E19" s="68" t="s">
         <v>5</v>
@@ -39120,13 +39095,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="68" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C20" s="69" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D20" s="70" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E20" s="68" t="s">
         <v>5</v>
@@ -39159,13 +39134,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C21" s="69" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D21" s="70" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E21" s="68" t="s">
         <v>5</v>
@@ -39198,13 +39173,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C22" s="69" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D22" s="70" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E22" s="68" t="s">
         <v>5</v>
@@ -39237,13 +39212,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C23" s="69" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D23" s="70" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E23" s="68" t="s">
         <v>5</v>
@@ -39276,13 +39251,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="68" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C24" s="69" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D24" s="70" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E24" s="68" t="s">
         <v>5</v>
@@ -39315,13 +39290,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="68" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C25" s="69" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D25" s="74" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E25" s="68" t="s">
         <v>5</v>
@@ -39354,13 +39329,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="68" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C26" s="69" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D26" s="70" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E26" s="68" t="s">
         <v>5</v>
@@ -39393,13 +39368,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="76" t="s">
+        <v>405</v>
+      </c>
+      <c r="C27" s="77" t="s">
         <v>408</v>
       </c>
-      <c r="C27" s="77" t="s">
-        <v>411</v>
-      </c>
       <c r="D27" s="78" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E27" s="68" t="s">
         <v>5</v>
@@ -39432,13 +39407,13 @@
         <v>13</v>
       </c>
       <c r="B28" s="80" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C28" s="81" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D28" s="82" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E28" s="80" t="s">
         <v>13</v>
@@ -39471,13 +39446,13 @@
         <v>13</v>
       </c>
       <c r="B29" s="84" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C29" s="85" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D29" s="86" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E29" s="84" t="s">
         <v>13</v>
@@ -39510,13 +39485,13 @@
         <v>13</v>
       </c>
       <c r="B30" s="84" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C30" s="85" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D30" s="86" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E30" s="84" t="s">
         <v>13</v>
@@ -39549,13 +39524,13 @@
         <v>13</v>
       </c>
       <c r="B31" s="84" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C31" s="85" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D31" s="86" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E31" s="84" t="s">
         <v>13</v>
@@ -39588,13 +39563,13 @@
         <v>13</v>
       </c>
       <c r="B32" s="84" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C32" s="85" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D32" s="86" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E32" s="84" t="s">
         <v>13</v>
@@ -39627,13 +39602,13 @@
         <v>13</v>
       </c>
       <c r="B33" s="84" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C33" s="85" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D33" s="86" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E33" s="84" t="s">
         <v>13</v>
@@ -39666,13 +39641,13 @@
         <v>13</v>
       </c>
       <c r="B34" s="84" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C34" s="85" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D34" s="86" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E34" s="84" t="s">
         <v>13</v>
@@ -39705,13 +39680,13 @@
         <v>13</v>
       </c>
       <c r="B35" s="84" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C35" s="85" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D35" s="86" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E35" s="84" t="s">
         <v>13</v>
@@ -39744,13 +39719,13 @@
         <v>13</v>
       </c>
       <c r="B36" s="84" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C36" s="85" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D36" s="87" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E36" s="84" t="s">
         <v>13</v>
@@ -39783,13 +39758,13 @@
         <v>13</v>
       </c>
       <c r="B37" s="84" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C37" s="85" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D37" s="86" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E37" s="84" t="s">
         <v>13</v>
@@ -39822,13 +39797,13 @@
         <v>13</v>
       </c>
       <c r="B38" s="84" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C38" s="85" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D38" s="86" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E38" s="84" t="s">
         <v>13</v>
@@ -39861,13 +39836,13 @@
         <v>13</v>
       </c>
       <c r="B39" s="84" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C39" s="85" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D39" s="86" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E39" s="84" t="s">
         <v>13</v>
@@ -39900,13 +39875,13 @@
         <v>13</v>
       </c>
       <c r="B40" s="84" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C40" s="85" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D40" s="86" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E40" s="84" t="s">
         <v>13</v>
@@ -39939,13 +39914,13 @@
         <v>13</v>
       </c>
       <c r="B41" s="84" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C41" s="85" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D41" s="86" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E41" s="84" t="s">
         <v>13</v>
@@ -39978,13 +39953,13 @@
         <v>13</v>
       </c>
       <c r="B42" s="84" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C42" s="85" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D42" s="86" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="E42" s="84" t="s">
         <v>13</v>
@@ -40017,13 +39992,13 @@
         <v>13</v>
       </c>
       <c r="B43" s="84" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C43" s="85" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D43" s="86" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E43" s="84" t="s">
         <v>13</v>
@@ -40056,13 +40031,13 @@
         <v>13</v>
       </c>
       <c r="B44" s="84" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C44" s="85" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D44" s="86" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E44" s="84" t="s">
         <v>13</v>
@@ -40095,13 +40070,13 @@
         <v>13</v>
       </c>
       <c r="B45" s="84" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C45" s="85" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D45" s="86" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E45" s="84" t="s">
         <v>13</v>
@@ -40134,13 +40109,13 @@
         <v>13</v>
       </c>
       <c r="B46" s="84" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C46" s="85" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D46" s="86" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E46" s="84" t="s">
         <v>13</v>
@@ -40173,13 +40148,13 @@
         <v>13</v>
       </c>
       <c r="B47" s="84" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C47" s="85" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D47" s="86" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E47" s="84" t="s">
         <v>13</v>
@@ -40212,13 +40187,13 @@
         <v>13</v>
       </c>
       <c r="B48" s="89" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C48" s="90" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D48" s="91" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E48" s="89" t="s">
         <v>13</v>
@@ -40251,13 +40226,13 @@
         <v>7</v>
       </c>
       <c r="B49" s="92" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C49" s="93" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="E49" s="92" t="s">
         <v>7</v>
@@ -40290,13 +40265,13 @@
         <v>7</v>
       </c>
       <c r="B50" s="92" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C50" s="93" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E50" s="92" t="s">
         <v>7</v>
@@ -40329,13 +40304,13 @@
         <v>7</v>
       </c>
       <c r="B51" s="92" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C51" s="92" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E51" s="92" t="s">
         <v>7</v>
@@ -40368,13 +40343,13 @@
         <v>7</v>
       </c>
       <c r="B52" s="92" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C52" s="92" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E52" s="92" t="s">
         <v>7</v>
@@ -40407,13 +40382,13 @@
         <v>7</v>
       </c>
       <c r="B53" s="92" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C53" s="92" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E53" s="92" t="s">
         <v>7</v>
@@ -40446,13 +40421,13 @@
         <v>7</v>
       </c>
       <c r="B54" s="92" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C54" s="92" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="E54" s="92" t="s">
         <v>7</v>
@@ -40485,13 +40460,13 @@
         <v>7</v>
       </c>
       <c r="B55" s="92" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C55" s="92" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E55" s="92" t="s">
         <v>7</v>
@@ -40524,13 +40499,13 @@
         <v>7</v>
       </c>
       <c r="B56" s="92" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C56" s="92" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E56" s="92" t="s">
         <v>7</v>
@@ -40563,13 +40538,13 @@
         <v>7</v>
       </c>
       <c r="B57" s="94" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C57" s="94" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D57" s="95" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E57" s="94" t="s">
         <v>11</v>
@@ -40602,13 +40577,13 @@
         <v>7</v>
       </c>
       <c r="B58" s="94" t="s">
+        <v>471</v>
+      </c>
+      <c r="C58" s="94" t="s">
         <v>474</v>
       </c>
-      <c r="C58" s="94" t="s">
-        <v>477</v>
-      </c>
       <c r="D58" s="95" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E58" s="94" t="s">
         <v>11</v>
@@ -40641,13 +40616,13 @@
         <v>7</v>
       </c>
       <c r="B59" s="94" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C59" s="94" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D59" s="95" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E59" s="94" t="s">
         <v>11</v>
@@ -40680,13 +40655,13 @@
         <v>7</v>
       </c>
       <c r="B60" s="92" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C60" s="92" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E60" s="92" t="s">
         <v>7</v>
@@ -40719,13 +40694,13 @@
         <v>7</v>
       </c>
       <c r="B61" s="92" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C61" s="92" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E61" s="92" t="s">
         <v>7</v>
@@ -40758,13 +40733,13 @@
         <v>7</v>
       </c>
       <c r="B62" s="96" t="s">
+        <v>480</v>
+      </c>
+      <c r="C62" s="96" t="s">
         <v>483</v>
       </c>
-      <c r="C62" s="96" t="s">
-        <v>486</v>
-      </c>
       <c r="D62" s="97" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E62" s="96" t="s">
         <v>7</v>
@@ -40797,13 +40772,13 @@
         <v>7</v>
       </c>
       <c r="B63" s="92" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C63" s="92" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D63" s="98" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="E63" s="92" t="s">
         <v>7</v>
@@ -40836,13 +40811,13 @@
         <v>7</v>
       </c>
       <c r="B64" s="92" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C64" s="92" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E64" s="92" t="s">
         <v>7</v>
@@ -40875,13 +40850,13 @@
         <v>7</v>
       </c>
       <c r="B65" s="92" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C65" s="92" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E65" s="92" t="s">
         <v>7</v>
@@ -40914,13 +40889,13 @@
         <v>7</v>
       </c>
       <c r="B66" s="92" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C66" s="92" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E66" s="92" t="s">
         <v>7</v>
@@ -40953,13 +40928,13 @@
         <v>7</v>
       </c>
       <c r="B67" s="92" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C67" s="92" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D67" s="98" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E67" s="92" t="s">
         <v>7</v>
@@ -40992,13 +40967,13 @@
         <v>7</v>
       </c>
       <c r="B68" s="92" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C68" s="99" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="E68" s="92" t="s">
         <v>7</v>
@@ -41031,13 +41006,13 @@
         <v>7</v>
       </c>
       <c r="B69" s="92" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C69" s="92" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="E69" s="92" t="s">
         <v>7</v>
@@ -41070,13 +41045,13 @@
         <v>7</v>
       </c>
       <c r="B70" s="92" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C70" s="99" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="E70" s="92" t="s">
         <v>7</v>
@@ -41109,13 +41084,13 @@
         <v>7</v>
       </c>
       <c r="B71" s="92" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C71" s="99" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E71" s="92" t="s">
         <v>7</v>
@@ -41148,13 +41123,13 @@
         <v>7</v>
       </c>
       <c r="B72" s="92" t="s">
+        <v>502</v>
+      </c>
+      <c r="C72" s="99" t="s">
         <v>505</v>
       </c>
-      <c r="C72" s="99" t="s">
-        <v>508</v>
-      </c>
       <c r="D72" s="14" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E72" s="92" t="s">
         <v>7</v>
@@ -41187,13 +41162,13 @@
         <v>7</v>
       </c>
       <c r="B73" s="92" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C73" s="99" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="E73" s="92" t="s">
         <v>7</v>
@@ -41226,13 +41201,13 @@
         <v>7</v>
       </c>
       <c r="B74" s="92" t="s">
+        <v>507</v>
+      </c>
+      <c r="C74" s="92" t="s">
         <v>510</v>
       </c>
-      <c r="C74" s="92" t="s">
-        <v>513</v>
-      </c>
       <c r="D74" s="14" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E74" s="92" t="s">
         <v>7</v>
@@ -41265,13 +41240,13 @@
         <v>7</v>
       </c>
       <c r="B75" s="92" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C75" s="92" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E75" s="92" t="s">
         <v>7</v>
@@ -41304,13 +41279,13 @@
         <v>7</v>
       </c>
       <c r="B76" s="92" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C76" s="92" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E76" s="92" t="s">
         <v>7</v>
@@ -41343,13 +41318,13 @@
         <v>7</v>
       </c>
       <c r="B77" s="92" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C77" s="92" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E77" s="92" t="s">
         <v>7</v>
@@ -41382,13 +41357,13 @@
         <v>7</v>
       </c>
       <c r="B78" s="92" t="s">
+        <v>516</v>
+      </c>
+      <c r="C78" s="92" t="s">
         <v>519</v>
       </c>
-      <c r="C78" s="92" t="s">
-        <v>522</v>
-      </c>
       <c r="D78" s="14" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E78" s="92" t="s">
         <v>7</v>
@@ -41421,13 +41396,13 @@
         <v>7</v>
       </c>
       <c r="B79" s="96" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C79" s="96" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D79" s="97" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E79" s="96" t="s">
         <v>7</v>
@@ -41460,13 +41435,13 @@
         <v>9</v>
       </c>
       <c r="B80" s="100" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C80" s="100" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D80" s="101" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="E80" s="100" t="s">
         <v>9</v>
@@ -41499,13 +41474,13 @@
         <v>9</v>
       </c>
       <c r="B81" s="100" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C81" s="100" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D81" s="101" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E81" s="100" t="s">
         <v>9</v>
@@ -41538,13 +41513,13 @@
         <v>9</v>
       </c>
       <c r="B82" s="100" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C82" s="100" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D82" s="101" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E82" s="100" t="s">
         <v>9</v>
@@ -41577,13 +41552,13 @@
         <v>9</v>
       </c>
       <c r="B83" s="100" t="s">
+        <v>528</v>
+      </c>
+      <c r="C83" s="100" t="s">
         <v>531</v>
       </c>
-      <c r="C83" s="100" t="s">
-        <v>534</v>
-      </c>
       <c r="D83" s="101" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E83" s="100" t="s">
         <v>9</v>
@@ -41616,13 +41591,13 @@
         <v>9</v>
       </c>
       <c r="B84" s="100" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C84" s="100" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D84" s="101" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E84" s="100" t="s">
         <v>9</v>
@@ -41655,13 +41630,13 @@
         <v>9</v>
       </c>
       <c r="B85" s="100" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C85" s="100" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D85" s="101" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E85" s="100" t="s">
         <v>9</v>
@@ -41694,13 +41669,13 @@
         <v>9</v>
       </c>
       <c r="B86" s="100" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C86" s="100" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D86" s="101" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E86" s="100" t="s">
         <v>9</v>
@@ -41733,13 +41708,13 @@
         <v>9</v>
       </c>
       <c r="B87" s="100" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C87" s="100" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D87" s="101" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E87" s="100" t="s">
         <v>9</v>
@@ -41772,13 +41747,13 @@
         <v>9</v>
       </c>
       <c r="B88" s="100" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C88" s="100" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D88" s="102" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E88" s="100" t="s">
         <v>9</v>
@@ -41811,13 +41786,13 @@
         <v>9</v>
       </c>
       <c r="B89" s="100" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C89" s="100" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D89" s="101" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="E89" s="100" t="s">
         <v>9</v>
@@ -41850,13 +41825,13 @@
         <v>9</v>
       </c>
       <c r="B90" s="100" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C90" s="100" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D90" s="101" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E90" s="100" t="s">
         <v>9</v>
@@ -41889,13 +41864,13 @@
         <v>9</v>
       </c>
       <c r="B91" s="100" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C91" s="100" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D91" s="101" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E91" s="100" t="s">
         <v>9</v>
@@ -41928,13 +41903,13 @@
         <v>9</v>
       </c>
       <c r="B92" s="103" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C92" s="103" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="D92" s="104" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E92" s="103" t="s">
         <v>9</v>
@@ -41967,13 +41942,13 @@
         <v>9</v>
       </c>
       <c r="B93" s="103" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C93" s="103" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D93" s="104" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E93" s="103" t="s">
         <v>9</v>
@@ -42006,13 +41981,13 @@
         <v>9</v>
       </c>
       <c r="B94" s="103" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C94" s="103" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D94" s="104" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E94" s="103" t="s">
         <v>9</v>
@@ -42045,13 +42020,13 @@
         <v>9</v>
       </c>
       <c r="B95" s="103" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C95" s="103" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D95" s="104" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E95" s="103" t="s">
         <v>9</v>
@@ -42084,13 +42059,13 @@
         <v>9</v>
       </c>
       <c r="B96" s="103" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C96" s="103" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D96" s="104" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E96" s="103" t="s">
         <v>9</v>
@@ -42123,13 +42098,13 @@
         <v>9</v>
       </c>
       <c r="B97" s="103" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C97" s="103" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D97" s="104" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="E97" s="103" t="s">
         <v>9</v>
@@ -42162,13 +42137,13 @@
         <v>9</v>
       </c>
       <c r="B98" s="103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C98" s="103" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D98" s="104" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E98" s="103" t="s">
         <v>9</v>
@@ -42201,13 +42176,13 @@
         <v>9</v>
       </c>
       <c r="B99" s="103" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C99" s="103" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D99" s="104" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E99" s="103" t="s">
         <v>9</v>
@@ -42240,13 +42215,13 @@
         <v>9</v>
       </c>
       <c r="B100" s="103" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C100" s="103" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="D100" s="104" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E100" s="103" t="s">
         <v>9</v>
@@ -42279,13 +42254,13 @@
         <v>9</v>
       </c>
       <c r="B101" s="103" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C101" s="103" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="D101" s="104" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E101" s="103" t="s">
         <v>9</v>
@@ -42318,13 +42293,13 @@
         <v>9</v>
       </c>
       <c r="B102" s="103" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C102" s="103" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D102" s="104" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E102" s="103" t="s">
         <v>9</v>
@@ -42357,13 +42332,13 @@
         <v>9</v>
       </c>
       <c r="B103" s="105" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C103" s="105" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D103" s="106" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E103" s="105" t="s">
         <v>9</v>
@@ -42396,13 +42371,13 @@
         <v>11</v>
       </c>
       <c r="B104" s="64" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C104" s="64" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D104" s="107" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E104" s="64" t="s">
         <v>11</v>
@@ -42435,13 +42410,13 @@
         <v>11</v>
       </c>
       <c r="B105" s="64" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C105" s="64" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D105" s="107" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E105" s="64" t="s">
         <v>11</v>
@@ -42474,13 +42449,13 @@
         <v>11</v>
       </c>
       <c r="B106" s="64" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C106" s="64" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D106" s="107" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E106" s="64" t="s">
         <v>11</v>
@@ -42513,13 +42488,13 @@
         <v>11</v>
       </c>
       <c r="B107" s="64" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C107" s="64" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D107" s="107" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E107" s="64" t="s">
         <v>11</v>
@@ -42552,13 +42527,13 @@
         <v>11</v>
       </c>
       <c r="B108" s="64" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C108" s="64" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D108" s="107" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E108" s="64" t="s">
         <v>11</v>
@@ -42591,13 +42566,13 @@
         <v>11</v>
       </c>
       <c r="B109" s="64" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C109" s="64" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D109" s="107" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E109" s="64" t="s">
         <v>11</v>
@@ -42630,13 +42605,13 @@
         <v>11</v>
       </c>
       <c r="B110" s="64" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C110" s="64" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D110" s="107" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E110" s="64" t="s">
         <v>11</v>
@@ -42669,13 +42644,13 @@
         <v>11</v>
       </c>
       <c r="B111" s="64" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C111" s="64" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D111" s="107" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E111" s="64" t="s">
         <v>11</v>
@@ -42708,13 +42683,13 @@
         <v>11</v>
       </c>
       <c r="B112" s="64" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C112" s="64" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D112" s="107" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E112" s="64" t="s">
         <v>11</v>
@@ -42747,13 +42722,13 @@
         <v>11</v>
       </c>
       <c r="B113" s="64" t="s">
+        <v>591</v>
+      </c>
+      <c r="C113" s="64" t="s">
         <v>594</v>
       </c>
-      <c r="C113" s="64" t="s">
-        <v>597</v>
-      </c>
       <c r="D113" s="107" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E113" s="64" t="s">
         <v>11</v>
@@ -42786,13 +42761,13 @@
         <v>11</v>
       </c>
       <c r="B114" s="64" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C114" s="64" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D114" s="107" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E114" s="64" t="s">
         <v>11</v>
@@ -42825,13 +42800,13 @@
         <v>11</v>
       </c>
       <c r="B115" s="64" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C115" s="64" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D115" s="107" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E115" s="64" t="s">
         <v>11</v>
@@ -42864,13 +42839,13 @@
         <v>11</v>
       </c>
       <c r="B116" s="64" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C116" s="64" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D116" s="107" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E116" s="64" t="s">
         <v>11</v>
@@ -42903,13 +42878,13 @@
         <v>11</v>
       </c>
       <c r="B117" s="64" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C117" s="64" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D117" s="107" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E117" s="64" t="s">
         <v>11</v>
@@ -42942,13 +42917,13 @@
         <v>11</v>
       </c>
       <c r="B118" s="64" t="s">
+        <v>602</v>
+      </c>
+      <c r="C118" s="64" t="s">
         <v>605</v>
       </c>
-      <c r="C118" s="64" t="s">
-        <v>608</v>
-      </c>
       <c r="D118" s="107" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E118" s="64" t="s">
         <v>11</v>
@@ -42981,13 +42956,13 @@
         <v>11</v>
       </c>
       <c r="B119" s="64" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C119" s="64" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D119" s="107" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E119" s="64" t="s">
         <v>11</v>
@@ -43020,13 +42995,13 @@
         <v>11</v>
       </c>
       <c r="B120" s="64" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C120" s="64" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D120" s="107" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E120" s="64" t="s">
         <v>11</v>
@@ -43059,13 +43034,13 @@
         <v>11</v>
       </c>
       <c r="B121" s="64" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C121" s="64" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D121" s="107" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E121" s="64" t="s">
         <v>11</v>
@@ -43098,13 +43073,13 @@
         <v>11</v>
       </c>
       <c r="B122" s="64" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C122" s="64" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="D122" s="107" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E122" s="64" t="s">
         <v>11</v>
@@ -43137,13 +43112,13 @@
         <v>11</v>
       </c>
       <c r="B123" s="64" t="s">
+        <v>613</v>
+      </c>
+      <c r="C123" s="64" t="s">
         <v>616</v>
       </c>
-      <c r="C123" s="64" t="s">
-        <v>619</v>
-      </c>
       <c r="D123" s="107" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E123" s="64" t="s">
         <v>11</v>
@@ -43176,13 +43151,13 @@
         <v>11</v>
       </c>
       <c r="B124" s="64" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C124" s="64" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D124" s="107" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E124" s="64" t="s">
         <v>11</v>
@@ -43215,13 +43190,13 @@
         <v>11</v>
       </c>
       <c r="B125" s="64" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C125" s="64" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D125" s="107" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E125" s="64" t="s">
         <v>11</v>
@@ -43254,13 +43229,13 @@
         <v>11</v>
       </c>
       <c r="B126" s="64" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C126" s="64" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D126" s="107" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E126" s="64" t="s">
         <v>11</v>
@@ -43293,13 +43268,13 @@
         <v>11</v>
       </c>
       <c r="B127" s="64" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C127" s="64" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D127" s="107" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E127" s="64" t="s">
         <v>11</v>
@@ -43332,13 +43307,13 @@
         <v>11</v>
       </c>
       <c r="B128" s="64" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C128" s="64" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D128" s="107" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E128" s="64" t="s">
         <v>11</v>
@@ -43371,13 +43346,13 @@
         <v>11</v>
       </c>
       <c r="B129" s="64" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C129" s="64" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D129" s="107" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E129" s="64" t="s">
         <v>11</v>
@@ -43410,13 +43385,13 @@
         <v>11</v>
       </c>
       <c r="B130" s="64" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C130" s="64" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D130" s="107" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="E130" s="64" t="s">
         <v>11</v>
@@ -43449,13 +43424,13 @@
         <v>11</v>
       </c>
       <c r="B131" s="64" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C131" s="64" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D131" s="107" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="E131" s="64" t="s">
         <v>11</v>
@@ -43488,13 +43463,13 @@
         <v>11</v>
       </c>
       <c r="B132" s="64" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C132" s="64" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D132" s="107" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="E132" s="64" t="s">
         <v>11</v>
@@ -43527,13 +43502,13 @@
         <v>11</v>
       </c>
       <c r="B133" s="64" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C133" s="64" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D133" s="107" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E133" s="64" t="s">
         <v>11</v>
@@ -68501,26 +68476,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update quiz for new tags
</commit_message>
<xml_diff>
--- a/lost-and-found/parser-quiz/input.xlsx
+++ b/lost-and-found/parser-quiz/input.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="677">
   <si>
     <t>ID Bloco</t>
   </si>
@@ -405,8 +405,8 @@
     <t>Você pretende incluir essa criança e/ou adolescente em seu plano de fuga?</t>
   </si>
   <si>
-    <t>S: R38, P14
-N: R39, R40, P14
+    <t>S: R38, P14, T3
+N: R39, R40, P14, T4
 T: R41, P14, T2</t>
   </si>
   <si>
@@ -477,8 +477,8 @@
   </si>
   <si>
     <t>"Trabalho e tenho liberdade com o meu dinheiro.": R60, P20
-“Não trabalho, mas recebo benefício/ pensão.”: R61, P20
-"Dependo financeiramente/ ele controla meu dinheiro.": R62, P20</t>
+“Não trabalho, mas recebo benefício/ pensão.”: R61, P20, T5
+"Dependo financeiramente/ ele controla meu dinheiro.": R62, P20, T6</t>
   </si>
   <si>
     <t>P20</t>
@@ -503,7 +503,7 @@
     <t>P21</t>
   </si>
   <si>
-    <t>Você mora com  o agressor?</t>
+    <t>Você mora com o agressor?</t>
   </si>
   <si>
     <t>S: R77, R78, R79, P22
@@ -558,7 +558,7 @@
     <t xml:space="preserve">Você possui alguma deficiência física e/ou intelectual?  </t>
   </si>
   <si>
-    <t>S: R94, R95, P27
+    <t>S: R94, R95, P27, T7
 N: P27</t>
   </si>
   <si>
@@ -569,7 +569,7 @@
   </si>
   <si>
     <t>S: R96, R97, R98, PQ
-N: R98, PQ</t>
+N: R98, PQ, T8</t>
   </si>
   <si>
     <t>P999</t>
@@ -2165,10 +2165,43 @@
     <t>DESCRICAO</t>
   </si>
   <si>
-    <t>Quis saber havia no estado/cidade serviços de acolhimento</t>
+    <t>Quis saber se havia no estado/cidade serviços de acolhimento</t>
+  </si>
+  <si>
+    <t>R5, R6, R7</t>
   </si>
   <si>
     <t>Talvez pretende incluir uma criança e/ou adolescente no plano de fuga</t>
+  </si>
+  <si>
+    <t>Sim, pretende incluir uma criança e/ou adolescente no plano de fuga</t>
+  </si>
+  <si>
+    <t>Não pretende incluir uma criança e/ou adolescente no plano de fuga</t>
+  </si>
+  <si>
+    <t>R39, R40</t>
+  </si>
+  <si>
+    <t>Sim, possuí renda (trabalho ou benefício)</t>
+  </si>
+  <si>
+    <t>R60, R61</t>
+  </si>
+  <si>
+    <t>Depende financeiramente do agressor/tem seu dinheiro controlado por ele</t>
+  </si>
+  <si>
+    <t>Tem deficiência física ou intelectual</t>
+  </si>
+  <si>
+    <t>R94, R95</t>
+  </si>
+  <si>
+    <t>Está grávida</t>
+  </si>
+  <si>
+    <t>R96, R97, R98</t>
   </si>
   <si>
     <t>SIM_LIMPA_MF</t>
@@ -2187,7 +2220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2341,6 +2374,12 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -2465,7 +2504,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="163">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2935,10 +2974,22 @@
     <xf borderId="11" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -68931,13 +68982,27 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="20.88"/>
+    <col customWidth="1" min="2" max="2" width="57.0"/>
+    <col customWidth="1" min="5" max="5" width="19.5"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="157" t="s">
         <v>658</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="157" t="s">
         <v>659</v>
+      </c>
+      <c r="C1" s="158" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="158" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="159" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="2">
@@ -68947,29 +69012,149 @@
       <c r="B2" s="7" t="s">
         <v>660</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
         <v>362</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>661</v>
+        <v>662</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>662</v>
+        <v>364</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>663</v>
       </c>
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="157" t="s">
+      <c r="A5" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="B5" s="158" t="s">
+      <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="160" t="s">
         <v>665</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="161" t="s">
+        <v>675</v>
+      </c>
+      <c r="B11" s="162" t="s">
+        <v>676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>